<commit_message>
Tests: Implemented reading from Excel
</commit_message>
<xml_diff>
--- a/Core.Tests/Reference/Simple-ProRata.xlsx
+++ b/Core.Tests/Reference/Simple-ProRata.xlsx
@@ -9,14 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24105" windowHeight="14310" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24105" windowHeight="14310"/>
   </bookViews>
   <sheets>
-    <sheet name="Input" sheetId="1" r:id="rId1"/>
-    <sheet name="AmortisationSummary" sheetId="4" r:id="rId2"/>
-    <sheet name="Amortisation-Home" sheetId="2" r:id="rId3"/>
-    <sheet name="Amortisation-Vehicle" sheetId="5" r:id="rId4"/>
-    <sheet name="Amortisation-CreditCard" sheetId="6" r:id="rId5"/>
+    <sheet name="Input" sheetId="7" r:id="rId1"/>
+    <sheet name="Creditors" sheetId="1" r:id="rId2"/>
+    <sheet name="Amortisation-Summary" sheetId="4" r:id="rId3"/>
+    <sheet name="Amortisation-Home" sheetId="2" r:id="rId4"/>
+    <sheet name="Amortisation-Vehicle" sheetId="5" r:id="rId5"/>
+    <sheet name="Amortisation-CreditCard" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -524,10 +525,76 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U5"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>5000</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.03</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R5"/>
+  <sheetViews>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:U1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,7 +620,7 @@
     <col min="21" max="21" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -587,35 +654,8 @@
       <c r="K1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -636,20 +676,13 @@
         <v>0.5714285714285714</v>
       </c>
       <c r="K2">
-        <f>J2*N$2</f>
+        <f>J2*Input!B$2</f>
         <v>2857.1428571428569</v>
       </c>
-      <c r="N2">
-        <v>5000</v>
-      </c>
-      <c r="Q2" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="R2" s="1">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -670,11 +703,11 @@
         <v>0.2857142857142857</v>
       </c>
       <c r="K3">
-        <f>J3*N$2</f>
+        <f>J3*Input!B$2</f>
         <v>1428.5714285714284</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -695,11 +728,11 @@
         <v>0.14285714285714285</v>
       </c>
       <c r="K4">
-        <f>J4*N$2</f>
+        <f>J4*Input!B$2</f>
         <v>714.28571428571422</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="J5">
         <f>SUM(J2:J4)</f>
         <v>1</v>
@@ -715,12 +748,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -771,7 +804,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <f>Input!N$2</f>
+        <f>Input!B$2</f>
         <v>5000</v>
       </c>
       <c r="D2">
@@ -779,7 +812,7 @@
         <v>4750</v>
       </c>
       <c r="G2">
-        <f>C2*Input!Q$2</f>
+        <f>C2*Input!E$2</f>
         <v>250</v>
       </c>
       <c r="H2">
@@ -797,7 +830,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <f>Input!N$2</f>
+        <f>Input!B$2</f>
         <v>5000</v>
       </c>
       <c r="D3">
@@ -805,7 +838,7 @@
         <v>4750</v>
       </c>
       <c r="G3">
-        <f>C3*Input!Q$2</f>
+        <f>C3*Input!E$2</f>
         <v>250</v>
       </c>
       <c r="H3">
@@ -823,7 +856,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <f>Input!N$2</f>
+        <f>Input!B$2</f>
         <v>5000</v>
       </c>
       <c r="D4">
@@ -831,7 +864,7 @@
         <v>4750</v>
       </c>
       <c r="G4">
-        <f>C4*Input!Q$2</f>
+        <f>C4*Input!E$2</f>
         <v>250</v>
       </c>
       <c r="H4">
@@ -849,7 +882,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <f>Input!N$2</f>
+        <f>Input!B$2</f>
         <v>5000</v>
       </c>
       <c r="D5">
@@ -857,7 +890,7 @@
         <v>2837.9633420758942</v>
       </c>
       <c r="G5">
-        <f>C5*Input!Q$2</f>
+        <f>C5*Input!E$2</f>
         <v>250</v>
       </c>
       <c r="H5">
@@ -875,7 +908,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <f>Input!N$2</f>
+        <f>Input!B$2</f>
         <v>5000</v>
       </c>
       <c r="D6">
@@ -883,7 +916,7 @@
         <v>0</v>
       </c>
       <c r="G6">
-        <f>C6*Input!Q$2</f>
+        <f>C6*Input!E$2</f>
         <v>250</v>
       </c>
       <c r="H6">
@@ -897,7 +930,7 @@
         <v>6</v>
       </c>
       <c r="C7">
-        <f>Input!N$2</f>
+        <f>Input!B$2</f>
         <v>5000</v>
       </c>
       <c r="D7">
@@ -905,7 +938,7 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <f>C7*Input!Q$2</f>
+        <f>C7*Input!E$2</f>
         <v>250</v>
       </c>
       <c r="H7">
@@ -919,7 +952,7 @@
         <v>7</v>
       </c>
       <c r="C8">
-        <f>Input!N$2</f>
+        <f>Input!B$2</f>
         <v>5000</v>
       </c>
       <c r="D8">
@@ -927,7 +960,7 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <f>C8*Input!Q$2</f>
+        <f>C8*Input!E$2</f>
         <v>250</v>
       </c>
       <c r="H8">
@@ -941,7 +974,7 @@
         <v>8</v>
       </c>
       <c r="C9">
-        <f>Input!N$2</f>
+        <f>Input!B$2</f>
         <v>5000</v>
       </c>
       <c r="D9">
@@ -949,7 +982,7 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <f>C9*Input!Q$2</f>
+        <f>C9*Input!E$2</f>
         <v>250</v>
       </c>
       <c r="H9">
@@ -963,7 +996,7 @@
         <v>9</v>
       </c>
       <c r="C10">
-        <f>Input!N$2</f>
+        <f>Input!B$2</f>
         <v>5000</v>
       </c>
       <c r="D10">
@@ -971,7 +1004,7 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <f>C10*Input!Q$2</f>
+        <f>C10*Input!E$2</f>
         <v>250</v>
       </c>
       <c r="H10">
@@ -985,7 +1018,7 @@
         <v>10</v>
       </c>
       <c r="C11">
-        <f>Input!N$2</f>
+        <f>Input!B$2</f>
         <v>5000</v>
       </c>
       <c r="D11">
@@ -993,7 +1026,7 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <f>C11*Input!Q$2</f>
+        <f>C11*Input!E$2</f>
         <v>250</v>
       </c>
       <c r="H11">
@@ -1007,11 +1040,11 @@
         <v>11</v>
       </c>
       <c r="C12">
-        <f>Input!N$2</f>
+        <f>Input!B$2</f>
         <v>5000</v>
       </c>
       <c r="G12">
-        <f>C12*Input!Q$2</f>
+        <f>C12*Input!E$2</f>
         <v>250</v>
       </c>
       <c r="H12">
@@ -1025,11 +1058,11 @@
         <v>12</v>
       </c>
       <c r="C13">
-        <f>Input!N$2</f>
+        <f>Input!B$2</f>
         <v>5000</v>
       </c>
       <c r="G13">
-        <f>C13*Input!Q$2</f>
+        <f>C13*Input!E$2</f>
         <v>250</v>
       </c>
       <c r="H13">
@@ -1043,11 +1076,11 @@
         <v>13</v>
       </c>
       <c r="C14">
-        <f>Input!N$2</f>
+        <f>Input!B$2</f>
         <v>5000</v>
       </c>
       <c r="G14">
-        <f>C14*Input!Q$2</f>
+        <f>C14*Input!E$2</f>
         <v>250</v>
       </c>
       <c r="H14">
@@ -1061,11 +1094,11 @@
         <v>14</v>
       </c>
       <c r="C15">
-        <f>Input!N$2</f>
+        <f>Input!B$2</f>
         <v>5000</v>
       </c>
       <c r="G15">
-        <f>C15*Input!Q$2</f>
+        <f>C15*Input!E$2</f>
         <v>250</v>
       </c>
       <c r="H15">
@@ -1079,11 +1112,11 @@
         <v>15</v>
       </c>
       <c r="C16">
-        <f>Input!N$2</f>
+        <f>Input!B$2</f>
         <v>5000</v>
       </c>
       <c r="G16">
-        <f>C16*Input!Q$2</f>
+        <f>C16*Input!E$2</f>
         <v>250</v>
       </c>
       <c r="H16">
@@ -1097,11 +1130,11 @@
         <v>16</v>
       </c>
       <c r="C17">
-        <f>Input!N$2</f>
+        <f>Input!B$2</f>
         <v>5000</v>
       </c>
       <c r="G17">
-        <f>C17*Input!Q$2</f>
+        <f>C17*Input!E$2</f>
         <v>250</v>
       </c>
       <c r="H17">
@@ -1115,11 +1148,11 @@
         <v>17</v>
       </c>
       <c r="C18">
-        <f>Input!N$2</f>
+        <f>Input!B$2</f>
         <v>5000</v>
       </c>
       <c r="G18">
-        <f>C18*Input!Q$2</f>
+        <f>C18*Input!E$2</f>
         <v>250</v>
       </c>
       <c r="H18">
@@ -1133,11 +1166,11 @@
         <v>18</v>
       </c>
       <c r="C19">
-        <f>Input!N$2</f>
+        <f>Input!B$2</f>
         <v>5000</v>
       </c>
       <c r="G19">
-        <f>C19*Input!Q$2</f>
+        <f>C19*Input!E$2</f>
         <v>250</v>
       </c>
       <c r="H19">
@@ -1151,11 +1184,11 @@
         <v>19</v>
       </c>
       <c r="C20">
-        <f>Input!N$2</f>
+        <f>Input!B$2</f>
         <v>5000</v>
       </c>
       <c r="G20">
-        <f>C20*Input!Q$2</f>
+        <f>C20*Input!E$2</f>
         <v>250</v>
       </c>
       <c r="H20">
@@ -1169,11 +1202,11 @@
         <v>20</v>
       </c>
       <c r="C21">
-        <f>Input!N$2</f>
+        <f>Input!B$2</f>
         <v>5000</v>
       </c>
       <c r="G21">
-        <f>C21*Input!Q$2</f>
+        <f>C21*Input!E$2</f>
         <v>250</v>
       </c>
       <c r="H21">
@@ -1187,11 +1220,11 @@
         <v>21</v>
       </c>
       <c r="C22">
-        <f>Input!N$2</f>
+        <f>Input!B$2</f>
         <v>5000</v>
       </c>
       <c r="G22">
-        <f>C22*Input!Q$2</f>
+        <f>C22*Input!E$2</f>
         <v>250</v>
       </c>
       <c r="H22">
@@ -1205,11 +1238,11 @@
         <v>22</v>
       </c>
       <c r="C23">
-        <f>Input!N$2</f>
+        <f>Input!B$2</f>
         <v>5000</v>
       </c>
       <c r="G23">
-        <f>C23*Input!Q$2</f>
+        <f>C23*Input!E$2</f>
         <v>250</v>
       </c>
       <c r="H23">
@@ -1223,11 +1256,11 @@
         <v>23</v>
       </c>
       <c r="C24">
-        <f>Input!N$2</f>
+        <f>Input!B$2</f>
         <v>5000</v>
       </c>
       <c r="G24">
-        <f>C24*Input!Q$2</f>
+        <f>C24*Input!E$2</f>
         <v>250</v>
       </c>
       <c r="H24">
@@ -1240,12 +1273,12 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="C25" s="4">
-        <f>Input!N$2</f>
-        <v>5000</v>
-      </c>
-      <c r="G25" s="4">
-        <f>C25*Input!Q$2</f>
+      <c r="C25">
+        <f>Input!B$2</f>
+        <v>5000</v>
+      </c>
+      <c r="G25">
+        <f>C25*Input!E$2</f>
         <v>250</v>
       </c>
       <c r="H25" s="4">
@@ -1259,11 +1292,11 @@
         <v>25</v>
       </c>
       <c r="C26">
-        <f>Input!N$2</f>
+        <f>Input!B$2</f>
         <v>5000</v>
       </c>
       <c r="G26">
-        <f>C26*Input!R$2</f>
+        <f>C26*Input!F$2</f>
         <v>150</v>
       </c>
       <c r="H26">
@@ -1277,11 +1310,11 @@
         <v>26</v>
       </c>
       <c r="C27">
-        <f>Input!N$2</f>
+        <f>Input!B$2</f>
         <v>5000</v>
       </c>
       <c r="G27">
-        <f>C27*Input!R$2</f>
+        <f>C27*Input!F$2</f>
         <v>150</v>
       </c>
       <c r="H27">
@@ -1295,11 +1328,11 @@
         <v>27</v>
       </c>
       <c r="C28">
-        <f>Input!N$2</f>
+        <f>Input!B$2</f>
         <v>5000</v>
       </c>
       <c r="G28">
-        <f>C28*Input!R$2</f>
+        <f>C28*Input!F$2</f>
         <v>150</v>
       </c>
       <c r="H28">
@@ -1313,11 +1346,11 @@
         <v>28</v>
       </c>
       <c r="C29">
-        <f>Input!N$2</f>
+        <f>Input!B$2</f>
         <v>5000</v>
       </c>
       <c r="G29">
-        <f>C29*Input!R$2</f>
+        <f>C29*Input!F$2</f>
         <v>150</v>
       </c>
       <c r="H29">
@@ -1331,11 +1364,11 @@
         <v>29</v>
       </c>
       <c r="C30">
-        <f>Input!N$2</f>
+        <f>Input!B$2</f>
         <v>5000</v>
       </c>
       <c r="G30">
-        <f>C30*Input!R$2</f>
+        <f>C30*Input!F$2</f>
         <v>150</v>
       </c>
       <c r="H30">
@@ -1349,11 +1382,11 @@
         <v>30</v>
       </c>
       <c r="C31">
-        <f>Input!N$2</f>
+        <f>Input!B$2</f>
         <v>5000</v>
       </c>
       <c r="G31">
-        <f>C31*Input!R$2</f>
+        <f>C31*Input!F$2</f>
         <v>150</v>
       </c>
       <c r="H31">
@@ -1367,11 +1400,11 @@
         <v>31</v>
       </c>
       <c r="C32">
-        <f>Input!N$2</f>
+        <f>Input!B$2</f>
         <v>5000</v>
       </c>
       <c r="G32">
-        <f>C32*Input!R$2</f>
+        <f>C32*Input!F$2</f>
         <v>150</v>
       </c>
       <c r="H32">
@@ -1385,11 +1418,11 @@
         <v>32</v>
       </c>
       <c r="C33">
-        <f>Input!N$2</f>
+        <f>Input!B$2</f>
         <v>5000</v>
       </c>
       <c r="G33">
-        <f>C33*Input!R$2</f>
+        <f>C33*Input!F$2</f>
         <v>150</v>
       </c>
       <c r="H33">
@@ -1403,11 +1436,11 @@
         <v>33</v>
       </c>
       <c r="C34">
-        <f>Input!N$2</f>
+        <f>Input!B$2</f>
         <v>5000</v>
       </c>
       <c r="G34">
-        <f>C34*Input!R$2</f>
+        <f>C34*Input!F$2</f>
         <v>150</v>
       </c>
       <c r="H34">
@@ -1421,11 +1454,11 @@
         <v>34</v>
       </c>
       <c r="C35">
-        <f>Input!N$2</f>
+        <f>Input!B$2</f>
         <v>5000</v>
       </c>
       <c r="G35">
-        <f>C35*Input!R$2</f>
+        <f>C35*Input!F$2</f>
         <v>150</v>
       </c>
       <c r="H35">
@@ -1439,11 +1472,11 @@
         <v>35</v>
       </c>
       <c r="C36">
-        <f>Input!N$2</f>
+        <f>Input!B$2</f>
         <v>5000</v>
       </c>
       <c r="G36">
-        <f>C36*Input!R$2</f>
+        <f>C36*Input!F$2</f>
         <v>150</v>
       </c>
       <c r="H36">
@@ -1457,11 +1490,11 @@
         <v>36</v>
       </c>
       <c r="C37">
-        <f>Input!N$2</f>
+        <f>Input!B$2</f>
         <v>5000</v>
       </c>
       <c r="G37">
-        <f>C37*Input!R$2</f>
+        <f>C37*Input!F$2</f>
         <v>150</v>
       </c>
       <c r="H37">
@@ -1475,11 +1508,11 @@
         <v>37</v>
       </c>
       <c r="C38">
-        <f>Input!N$2</f>
+        <f>Input!B$2</f>
         <v>5000</v>
       </c>
       <c r="G38">
-        <f>C38*Input!R$2</f>
+        <f>C38*Input!F$2</f>
         <v>150</v>
       </c>
       <c r="H38">
@@ -1493,11 +1526,11 @@
         <v>38</v>
       </c>
       <c r="C39">
-        <f>Input!N$2</f>
+        <f>Input!B$2</f>
         <v>5000</v>
       </c>
       <c r="G39">
-        <f>C39*Input!R$2</f>
+        <f>C39*Input!F$2</f>
         <v>150</v>
       </c>
       <c r="H39">
@@ -1511,11 +1544,11 @@
         <v>39</v>
       </c>
       <c r="C40">
-        <f>Input!N$2</f>
+        <f>Input!B$2</f>
         <v>5000</v>
       </c>
       <c r="G40">
-        <f>C40*Input!R$2</f>
+        <f>C40*Input!F$2</f>
         <v>150</v>
       </c>
       <c r="H40">
@@ -1529,11 +1562,11 @@
         <v>40</v>
       </c>
       <c r="C41">
-        <f>Input!N$2</f>
+        <f>Input!B$2</f>
         <v>5000</v>
       </c>
       <c r="G41">
-        <f>C41*Input!R$2</f>
+        <f>C41*Input!F$2</f>
         <v>150</v>
       </c>
       <c r="H41">
@@ -1547,11 +1580,11 @@
         <v>41</v>
       </c>
       <c r="C42">
-        <f>Input!N$2</f>
+        <f>Input!B$2</f>
         <v>5000</v>
       </c>
       <c r="G42">
-        <f>C42*Input!R$2</f>
+        <f>C42*Input!F$2</f>
         <v>150</v>
       </c>
       <c r="H42">
@@ -1565,11 +1598,11 @@
         <v>42</v>
       </c>
       <c r="C43">
-        <f>Input!N$2</f>
+        <f>Input!B$2</f>
         <v>5000</v>
       </c>
       <c r="G43">
-        <f>C43*Input!R$2</f>
+        <f>C43*Input!F$2</f>
         <v>150</v>
       </c>
       <c r="H43">
@@ -1583,11 +1616,11 @@
         <v>43</v>
       </c>
       <c r="C44">
-        <f>Input!N$2</f>
+        <f>Input!B$2</f>
         <v>5000</v>
       </c>
       <c r="G44">
-        <f>C44*Input!R$2</f>
+        <f>C44*Input!F$2</f>
         <v>150</v>
       </c>
       <c r="H44">
@@ -1600,7 +1633,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q6"/>
   <sheetViews>
@@ -1634,15 +1667,15 @@
         <v>29</v>
       </c>
       <c r="C1" s="2" t="str">
-        <f>Input!A1</f>
+        <f>Creditors!A1</f>
         <v>CreditorName</v>
       </c>
       <c r="D1" s="2" t="str">
-        <f>Input!B1</f>
+        <f>Creditors!B1</f>
         <v>CreditorType</v>
       </c>
       <c r="E1" s="2" t="str">
-        <f>Input!C1</f>
+        <f>Creditors!C1</f>
         <v>InterestRate</v>
       </c>
       <c r="F1" s="5" t="s">
@@ -1652,84 +1685,84 @@
         <v>31</v>
       </c>
       <c r="H1" s="2" t="str">
-        <f>Input!D1</f>
+        <f>Creditors!D1</f>
         <v>OriginalInstallment</v>
       </c>
       <c r="I1" s="5" t="str">
-        <f>Input!E1</f>
+        <f>Creditors!E1</f>
         <v>OutstandingBalance</v>
       </c>
       <c r="J1" s="2" t="str">
-        <f>Input!F1</f>
+        <f>Creditors!F1</f>
         <v>COB Date</v>
       </c>
       <c r="K1" s="2" t="str">
-        <f>Input!G1</f>
+        <f>Creditors!G1</f>
         <v>ServiceFees</v>
       </c>
       <c r="L1" s="2" t="str">
-        <f>Input!H1</f>
+        <f>Creditors!H1</f>
         <v>LinkedInsurance</v>
       </c>
       <c r="M1" s="2" t="str">
-        <f>Input!I1</f>
+        <f>Creditors!I1</f>
         <v>CustomInstallment</v>
       </c>
       <c r="N1" s="5" t="str">
-        <f>Input!J1</f>
+        <f>Creditors!J1</f>
         <v>ProRataPercentage</v>
       </c>
       <c r="O1" s="5" t="str">
-        <f>AmortisationSummary!H1</f>
+        <f>'Amortisation-Summary'!H1</f>
         <v>DistributableToCreditors</v>
       </c>
       <c r="P1" s="5" t="s">
         <v>34</v>
       </c>
       <c r="Q1" s="5" t="str">
-        <f>AmortisationSummary!I1</f>
+        <f>'Amortisation-Summary'!I1</f>
         <v>CreditorSurplus</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C2" t="str">
-        <f>Input!A2</f>
+        <f>Creditors!A2</f>
         <v>Home</v>
       </c>
       <c r="D2" t="str">
-        <f>Input!B2</f>
+        <f>Creditors!B2</f>
         <v>HL</v>
       </c>
       <c r="E2" s="7">
-        <f>Input!C2</f>
+        <f>Creditors!C2</f>
         <v>0.02</v>
       </c>
       <c r="H2">
-        <f>Input!D2</f>
+        <f>Creditors!D2</f>
         <v>4000</v>
       </c>
       <c r="I2">
-        <f>Input!E2</f>
+        <f>Creditors!E2</f>
         <v>10000</v>
       </c>
       <c r="J2">
-        <f>Input!F2</f>
+        <f>Creditors!F2</f>
         <v>0</v>
       </c>
       <c r="K2">
-        <f>Input!G2</f>
+        <f>Creditors!G2</f>
         <v>0</v>
       </c>
       <c r="L2">
-        <f>Input!H2</f>
+        <f>Creditors!H2</f>
         <v>0</v>
       </c>
       <c r="M2">
-        <f>Input!I2</f>
+        <f>Creditors!I2</f>
         <v>0</v>
       </c>
       <c r="N2">
-        <f>Input!J2</f>
+        <f>Creditors!J2</f>
         <v>0.5714285714285714</v>
       </c>
     </row>
@@ -1754,7 +1787,7 @@
         <v>0.5714285714285714</v>
       </c>
       <c r="O3">
-        <f>VLOOKUP(A3,AmortisationSummary!A:H, 8)</f>
+        <f>VLOOKUP(A3,'Amortisation-Summary'!A:H, 8)</f>
         <v>4750</v>
       </c>
     </row>
@@ -1780,7 +1813,7 @@
         <v>0.5714285714285714</v>
       </c>
       <c r="O4">
-        <f>VLOOKUP(A4,AmortisationSummary!A:H, 8)</f>
+        <f>VLOOKUP(A4,'Amortisation-Summary'!A:H, 8)</f>
         <v>4750</v>
       </c>
     </row>
@@ -1806,11 +1839,11 @@
         <v>0.5714285714285714</v>
       </c>
       <c r="O5">
-        <f>VLOOKUP(A5,AmortisationSummary!A:H, 8)</f>
+        <f>VLOOKUP(A5,'Amortisation-Summary'!A:H, 8)</f>
         <v>4750</v>
       </c>
       <c r="P5">
-        <f>Input!D2/(Input!D3+Input!D2)</f>
+        <f>Creditors!D2/(Creditors!D3+Creditors!D2)</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="Q5">
@@ -1839,7 +1872,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="O6">
-        <f>VLOOKUP(A6,AmortisationSummary!A:H, 8)</f>
+        <f>VLOOKUP(A6,'Amortisation-Summary'!A:H, 8)</f>
         <v>4750</v>
       </c>
     </row>
@@ -1848,7 +1881,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q6"/>
   <sheetViews>
@@ -1882,15 +1915,15 @@
         <v>29</v>
       </c>
       <c r="C1" s="2" t="str">
-        <f>Input!A1</f>
+        <f>Creditors!A1</f>
         <v>CreditorName</v>
       </c>
       <c r="D1" s="2" t="str">
-        <f>Input!B1</f>
+        <f>Creditors!B1</f>
         <v>CreditorType</v>
       </c>
       <c r="E1" s="2" t="str">
-        <f>Input!C1</f>
+        <f>Creditors!C1</f>
         <v>InterestRate</v>
       </c>
       <c r="F1" s="5" t="s">
@@ -1900,84 +1933,84 @@
         <v>31</v>
       </c>
       <c r="H1" s="2" t="str">
-        <f>Input!D1</f>
+        <f>Creditors!D1</f>
         <v>OriginalInstallment</v>
       </c>
       <c r="I1" s="5" t="str">
-        <f>Input!E1</f>
+        <f>Creditors!E1</f>
         <v>OutstandingBalance</v>
       </c>
       <c r="J1" s="2" t="str">
-        <f>Input!F1</f>
+        <f>Creditors!F1</f>
         <v>COB Date</v>
       </c>
       <c r="K1" s="2" t="str">
-        <f>Input!G1</f>
+        <f>Creditors!G1</f>
         <v>ServiceFees</v>
       </c>
       <c r="L1" s="2" t="str">
-        <f>Input!H1</f>
+        <f>Creditors!H1</f>
         <v>LinkedInsurance</v>
       </c>
       <c r="M1" s="2" t="str">
-        <f>Input!I1</f>
+        <f>Creditors!I1</f>
         <v>CustomInstallment</v>
       </c>
       <c r="N1" s="5" t="str">
-        <f>Input!J1</f>
+        <f>Creditors!J1</f>
         <v>ProRataPercentage</v>
       </c>
       <c r="O1" s="5" t="str">
-        <f>AmortisationSummary!H1</f>
+        <f>'Amortisation-Summary'!H1</f>
         <v>DistributableToCreditors</v>
       </c>
       <c r="P1" s="5" t="s">
         <v>34</v>
       </c>
       <c r="Q1" s="5" t="str">
-        <f>AmortisationSummary!I1</f>
+        <f>'Amortisation-Summary'!I1</f>
         <v>CreditorSurplus</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C2" t="str">
-        <f>Input!A3</f>
+        <f>Creditors!A3</f>
         <v>Vehicle</v>
       </c>
       <c r="D2" t="str">
-        <f>Input!B3</f>
+        <f>Creditors!B3</f>
         <v>VF</v>
       </c>
       <c r="E2" s="1">
-        <f>Input!C3</f>
+        <f>Creditors!C3</f>
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="H2">
-        <f>Input!D2</f>
+        <f>Creditors!D2</f>
         <v>4000</v>
       </c>
       <c r="I2">
-        <f>Input!E3</f>
+        <f>Creditors!E3</f>
         <v>5000</v>
       </c>
       <c r="J2">
-        <f>Input!F3</f>
+        <f>Creditors!F3</f>
         <v>0</v>
       </c>
       <c r="K2">
-        <f>Input!G3</f>
+        <f>Creditors!G3</f>
         <v>0</v>
       </c>
       <c r="L2">
-        <f>Input!H3</f>
+        <f>Creditors!H3</f>
         <v>0</v>
       </c>
       <c r="M2">
-        <f>Input!I3</f>
+        <f>Creditors!I3</f>
         <v>0</v>
       </c>
       <c r="N2">
-        <f>Input!J3</f>
+        <f>Creditors!J3</f>
         <v>0.2857142857142857</v>
       </c>
     </row>
@@ -2002,7 +2035,7 @@
         <v>0.2857142857142857</v>
       </c>
       <c r="O3">
-        <f>VLOOKUP(A3,AmortisationSummary!A:H, 8)</f>
+        <f>VLOOKUP(A3,'Amortisation-Summary'!A:H, 8)</f>
         <v>4750</v>
       </c>
     </row>
@@ -2028,7 +2061,7 @@
         <v>0.2857142857142857</v>
       </c>
       <c r="O4">
-        <f>VLOOKUP(A4,AmortisationSummary!A:H, 8)</f>
+        <f>VLOOKUP(A4,'Amortisation-Summary'!A:H, 8)</f>
         <v>4750</v>
       </c>
     </row>
@@ -2054,11 +2087,11 @@
         <v>0.2857142857142857</v>
       </c>
       <c r="O5">
-        <f>VLOOKUP(A5,AmortisationSummary!A:H, 8)</f>
+        <f>VLOOKUP(A5,'Amortisation-Summary'!A:H, 8)</f>
         <v>4750</v>
       </c>
       <c r="P5">
-        <f>Input!D3/(Input!D3+Input!D2)</f>
+        <f>Creditors!D3/(Creditors!D3+Creditors!D2)</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="Q5">
@@ -2087,7 +2120,7 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="O6">
-        <f>VLOOKUP(A6,AmortisationSummary!A:H, 8)</f>
+        <f>VLOOKUP(A6,'Amortisation-Summary'!A:H, 8)</f>
         <v>4750</v>
       </c>
     </row>
@@ -2096,7 +2129,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O5"/>
   <sheetViews>
@@ -2128,15 +2161,15 @@
         <v>29</v>
       </c>
       <c r="C1" s="2" t="str">
-        <f>Input!A1</f>
+        <f>Creditors!A1</f>
         <v>CreditorName</v>
       </c>
       <c r="D1" s="2" t="str">
-        <f>Input!B1</f>
+        <f>Creditors!B1</f>
         <v>CreditorType</v>
       </c>
       <c r="E1" s="2" t="str">
-        <f>Input!C1</f>
+        <f>Creditors!C1</f>
         <v>InterestRate</v>
       </c>
       <c r="F1" s="5" t="s">
@@ -2146,77 +2179,77 @@
         <v>31</v>
       </c>
       <c r="H1" s="2" t="str">
-        <f>Input!D1</f>
+        <f>Creditors!D1</f>
         <v>OriginalInstallment</v>
       </c>
       <c r="I1" s="5" t="str">
-        <f>Input!E1</f>
+        <f>Creditors!E1</f>
         <v>OutstandingBalance</v>
       </c>
       <c r="J1" s="2" t="str">
-        <f>Input!F1</f>
+        <f>Creditors!F1</f>
         <v>COB Date</v>
       </c>
       <c r="K1" s="2" t="str">
-        <f>Input!G1</f>
+        <f>Creditors!G1</f>
         <v>ServiceFees</v>
       </c>
       <c r="L1" s="2" t="str">
-        <f>Input!H1</f>
+        <f>Creditors!H1</f>
         <v>LinkedInsurance</v>
       </c>
       <c r="M1" s="2" t="str">
-        <f>Input!I1</f>
+        <f>Creditors!I1</f>
         <v>CustomInstallment</v>
       </c>
       <c r="N1" s="5" t="str">
-        <f>Input!J1</f>
+        <f>Creditors!J1</f>
         <v>ProRataPercentage</v>
       </c>
       <c r="O1" s="5" t="str">
-        <f>AmortisationSummary!H1</f>
+        <f>'Amortisation-Summary'!H1</f>
         <v>DistributableToCreditors</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C2" t="str">
-        <f>Input!A4</f>
+        <f>Creditors!A4</f>
         <v>CreditCard</v>
       </c>
       <c r="D2" t="str">
-        <f>Input!B4</f>
+        <f>Creditors!B4</f>
         <v>CO</v>
       </c>
       <c r="E2" s="1">
-        <f>Input!C4</f>
+        <f>Creditors!C4</f>
         <v>0.15</v>
       </c>
       <c r="H2">
-        <f>Input!D2</f>
+        <f>Creditors!D2</f>
         <v>4000</v>
       </c>
       <c r="I2">
-        <f>Input!E4</f>
+        <f>Creditors!E4</f>
         <v>2000</v>
       </c>
       <c r="J2">
-        <f>Input!F4</f>
+        <f>Creditors!F4</f>
         <v>0</v>
       </c>
       <c r="K2">
-        <f>Input!G4</f>
+        <f>Creditors!G4</f>
         <v>0</v>
       </c>
       <c r="L2">
-        <f>Input!H4</f>
+        <f>Creditors!H4</f>
         <v>0</v>
       </c>
       <c r="M2">
-        <f>Input!I4</f>
+        <f>Creditors!I4</f>
         <v>0</v>
       </c>
       <c r="N2">
-        <f>Input!J4</f>
+        <f>Creditors!J4</f>
         <v>0.14285714285714285</v>
       </c>
     </row>
@@ -2237,7 +2270,7 @@
         <v>1321.4285714285716</v>
       </c>
       <c r="O3">
-        <f>VLOOKUP(A3,AmortisationSummary!A:H, 8)</f>
+        <f>VLOOKUP(A3,'Amortisation-Summary'!A:H, 8)</f>
         <v>4750</v>
       </c>
     </row>
@@ -2259,7 +2292,7 @@
         <v>659.37500000000011</v>
       </c>
       <c r="O4">
-        <f>VLOOKUP(A4,AmortisationSummary!A:H, 8)</f>
+        <f>VLOOKUP(A4,'Amortisation-Summary'!A:H, 8)</f>
         <v>4750</v>
       </c>
     </row>
@@ -2281,7 +2314,7 @@
         <v>0</v>
       </c>
       <c r="O5">
-        <f>VLOOKUP(A5,AmortisationSummary!A:H, 8)</f>
+        <f>VLOOKUP(A5,'Amortisation-Summary'!A:H, 8)</f>
         <v>4750</v>
       </c>
     </row>

</xml_diff>

<commit_message>
First implementation. Simple-ProRata doesn't pass yet.
</commit_message>
<xml_diff>
--- a/Core.Tests/Reference/Simple-ProRata.xlsx
+++ b/Core.Tests/Reference/Simple-ProRata.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
   <si>
     <t>ContributionAmount</t>
   </si>
@@ -134,6 +134,12 @@
   </si>
   <si>
     <t>ProRataPercentageForSurplus</t>
+  </si>
+  <si>
+    <t>Strategy</t>
+  </si>
+  <si>
+    <t>ProRata</t>
   </si>
 </sst>
 </file>
@@ -525,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,7 +549,7 @@
     <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -571,8 +577,11 @@
       <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>5000</v>
       </c>
@@ -581,6 +590,9 @@
       </c>
       <c r="F2" s="1">
         <v>0.03</v>
+      </c>
+      <c r="J2" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -593,8 +605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:U1048576"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -753,7 +765,7 @@
   <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1630,6 +1642,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1638,7 +1651,7 @@
   <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1648,7 +1661,7 @@
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
     <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
@@ -1878,6 +1891,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2134,7 +2148,7 @@
   <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>